<commit_message>
updated PCB BOM file
</commit_message>
<xml_diff>
--- a/hardware/stm32_servo_controller/production/stm32_servo_controller_pcb_BOM_final.xlsx
+++ b/hardware/stm32_servo_controller/production/stm32_servo_controller_pcb_BOM_final.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
   <si>
     <t>Designator</t>
   </si>
@@ -28,7 +28,7 @@
     <t>LCSC Part #</t>
   </si>
   <si>
-    <t xml:space="preserve">Type </t>
+    <t xml:space="preserve">JLC assembly type </t>
   </si>
   <si>
     <t>C1, C10, C11, C18, C21, C22, C5, C6, C7, C9</t>
@@ -40,6 +40,9 @@
     <t>C14663</t>
   </si>
   <si>
+    <t>Basic</t>
+  </si>
+  <si>
     <t>C12, C13</t>
   </si>
   <si>
@@ -79,7 +82,7 @@
     <t>20pF</t>
   </si>
   <si>
-    <t>C1648</t>
+    <t>C325469</t>
   </si>
   <si>
     <t>D1, D4</t>
@@ -121,13 +124,16 @@
     <t>C516068</t>
   </si>
   <si>
+    <t>Extended</t>
+  </si>
+  <si>
     <t>FB1</t>
   </si>
   <si>
     <t>FerriteBead</t>
   </si>
   <si>
-    <t>C710378</t>
+    <t>C79382</t>
   </si>
   <si>
     <t>J3</t>
@@ -217,130 +223,130 @@
     <t>110K</t>
   </si>
   <si>
+    <t>C25805</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t>C22809</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>51K</t>
+  </si>
+  <si>
+    <t>C23196</t>
+  </si>
+  <si>
+    <t>R25, R26</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>0.5R</t>
+  </si>
+  <si>
+    <t>C28319</t>
+  </si>
+  <si>
+    <t>R6, R7</t>
+  </si>
+  <si>
+    <t>22R</t>
+  </si>
+  <si>
+    <t>C23345</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LQFP-48_7x7mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>STM32F103C8Tx</t>
+  </si>
+  <si>
+    <t>C8734</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C5180249</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>MT3608B</t>
+  </si>
+  <si>
+    <t>C19189893</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>LP5907MFX-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>C80670</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>HSOP-8-1EP_3.9x4.9mm_P1.27mm_EP2.3x2.3mm</t>
+  </si>
+  <si>
+    <t>IP2312</t>
+  </si>
+  <si>
+    <t>C605433</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>DW01</t>
+  </si>
+  <si>
     <t>C227441</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>15K</t>
-  </si>
-  <si>
-    <t>C22809</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>51K</t>
-  </si>
-  <si>
-    <t>C23196</t>
-  </si>
-  <si>
-    <t>R25, R26</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>C21190</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>0.5R</t>
-  </si>
-  <si>
-    <t>C28319</t>
-  </si>
-  <si>
-    <t>R6, R7</t>
-  </si>
-  <si>
-    <t>22R</t>
-  </si>
-  <si>
-    <t>C23345</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>LQFP-48_7x7mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>STM32F103C8Tx</t>
-  </si>
-  <si>
-    <t>C8734</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
-    <t>USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>C7519</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>MT3608B</t>
-  </si>
-  <si>
-    <t>C19189893</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>LP5907MFX-3.3</t>
-  </si>
-  <si>
-    <t>C80670</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>HSOP-8-1EP_3.9x4.9mm_P1.27mm_EP2.3x2.3mm</t>
-  </si>
-  <si>
-    <t>IP2312</t>
-  </si>
-  <si>
-    <t>C605433</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>DW01</t>
-  </si>
-  <si>
-    <t>DW01A</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
     <t>TSSOP-8_4.4x3mm_P0.65mm</t>
   </si>
   <si>
-    <t>AO8810</t>
-  </si>
-  <si>
-    <t>C21426</t>
+    <t>HL 8205A</t>
+  </si>
+  <si>
+    <t>C7499846</t>
   </si>
   <si>
     <t>U8</t>
@@ -358,13 +364,13 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>Crystal_SMD_HC49-4H</t>
+    <t>Crystal_HC49-4H</t>
   </si>
   <si>
     <t>8MHz</t>
   </si>
   <si>
-    <t>C259040</t>
+    <t>C21263</t>
   </si>
 </sst>
 </file>
@@ -379,18 +385,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,14 +405,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FFFFD966"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -429,9 +429,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -651,9 +655,11 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="37.25"/>
-    <col customWidth="1" min="2" max="2" width="30.5"/>
-    <col customWidth="1" min="3" max="3" width="14.63"/>
-    <col customWidth="1" min="4" max="4" width="14.25"/>
+    <col customWidth="1" min="2" max="2" width="40.13"/>
+    <col customWidth="1" min="3" max="3" width="18.0"/>
+    <col customWidth="1" min="4" max="4" width="22.38"/>
+    <col customWidth="1" min="5" max="5" width="15.5"/>
+    <col customWidth="1" min="6" max="6" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -672,604 +678,689 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>603.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>10.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1206.0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4">
+        <v>805.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>805.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="4">
         <v>1206.0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4">
+        <v>805.0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="4">
+        <v>603.0</v>
+      </c>
+      <c r="C24" s="3">
         <v>2.0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="D24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="4">
+        <v>805.0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="4">
         <v>603.0</v>
       </c>
-      <c r="C4" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2">
-        <v>805.0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="C26" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="3">
         <v>1.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2">
-        <v>805.0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="D27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="3">
         <v>1.0</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1206.0</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="D28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="3">
         <v>1.0</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2">
-        <v>805.0</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="D29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="3">
         <v>1.0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1">
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="3">
         <v>1.0</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="D31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="3">
         <v>1.0</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="D32" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="3">
         <v>1.0</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="D33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="3">
         <v>1.0</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="D34" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="3">
         <v>1.0</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="2">
-        <v>805.0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="2">
-        <v>603.0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F35" s="4"/>
+      <c r="D35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="6"/>
@@ -4131,6 +4222,11 @@
       <c r="B988" s="6"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F35">
+      <formula1>"Basic,Extended"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>